<commit_message>
TICKET-15991 PDB Upgrade (JAST Purchase_20220429.zip)
git-svn-id: svn+ssh://devteam/data/svn/tcijapp/Purchase/trunk@1932 ebf3080d-37d0-4b6c-8d7e-121e4dec3f32
</commit_message>
<xml_diff>
--- a/Purchase/App_Data/SupplierProduct.xlsx
+++ b/Purchase/App_Data/SupplierProduct.xlsx
@@ -374,7 +374,9 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -383,6 +385,7 @@
     <col min="6" max="6" width="50.75" customWidth="1"/>
     <col min="7" max="7" width="30.75" customWidth="1"/>
     <col min="8" max="8" width="25.75" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
     <col min="10" max="10" width="20.75" customWidth="1"/>
   </cols>
   <sheetData/>

</xml_diff>